<commit_message>
Más progreso en el front.
</commit_message>
<xml_diff>
--- a/Proyecto Final/abierto.xlsx
+++ b/Proyecto Final/abierto.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E7"/>
+  <dimension ref="A1:E14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -490,81 +490,81 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>192.168.247.12</t>
+          <t>192.168.247.18</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>2019-02-26</t>
+          <t>2019-08-21</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>2019-02-26</t>
+          <t>2020-02-19</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>3084</t>
+          <t>0</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>1344</t>
+          <t>0</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>192.168.247.11</t>
+          <t>192.168.247.12</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>2019-02-11</t>
+          <t>2019-02-26</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>2019-03-14</t>
+          <t>2019-02-26</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>1170</t>
+          <t>3084</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>495</t>
+          <t>1344</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>192.168.247.19</t>
+          <t>192.168.247.18</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>2019-02-19</t>
+          <t>2019-04-03</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>2019-02-19</t>
+          <t>2020-02-05</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>2554</t>
+          <t>0</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>334</t>
+          <t>0</t>
         </is>
       </c>
     </row>
@@ -576,49 +576,238 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>2019-02-12</t>
+          <t>2019-02-11</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>2019-03-06</t>
+          <t>2019-03-14</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>544518</t>
+          <t>1170</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>1881843</t>
+          <t>495</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
+          <t>192.168.247.20</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>2019-06-27</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>2020-10-08</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>8990</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>14372</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>192.168.247.19</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>2019-02-19</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>2019-02-19</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>2554</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>334</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>192.168.247.11</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>2019-02-12</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>2019-03-06</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>544518</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>1881843</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>192.168.247.19</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>2019-04-03</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>2020-10-13</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
           <t>192.168.247.18</t>
         </is>
       </c>
-      <c r="B7" t="inlineStr">
+      <c r="B11" t="inlineStr">
         <is>
           <t>2019-02-27</t>
         </is>
       </c>
-      <c r="C7" t="inlineStr">
+      <c r="C11" t="inlineStr">
         <is>
           <t>2020-02-04</t>
         </is>
       </c>
-      <c r="D7" t="inlineStr">
+      <c r="D11" t="inlineStr">
         <is>
           <t>2754</t>
         </is>
       </c>
-      <c r="E7" t="inlineStr">
+      <c r="E11" t="inlineStr">
         <is>
           <t>2432</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>192.168.247.15</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>2019-03-28</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>2019-03-28</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>16893</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>23855</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>192.168.247.16</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>2019-03-15</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>2019-05-02</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>192.168.247.18</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>2019-06-24</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>2019-06-24</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
     </row>

</xml_diff>